<commit_message>
added Onboarding with blood report and test data helper
</commit_message>
<xml_diff>
--- a/testData/testData.xlsx
+++ b/testData/testData.xlsx
@@ -5,6 +5,7 @@
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
     <sheet name="DiabeticRisk" sheetId="2" r:id="rId2"/>
+    <sheet name="OnboardingWithReport" sheetId="3" r:id="rId3"/>
   </sheets>
 </workbook>
 </file>
@@ -5047,4 +5048,134 @@
     <ignoredError numberStoredAsText="1" sqref="A1:F4"/>
   </ignoredErrors>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:Z4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>testCase</v>
+      </c>
+      <c r="B1" t="str">
+        <v>Email</v>
+      </c>
+      <c r="C1" t="str">
+        <v>Fullname</v>
+      </c>
+      <c r="D1" t="str">
+        <v>Username</v>
+      </c>
+      <c r="E1" t="str">
+        <v>Password</v>
+      </c>
+      <c r="F1" t="str">
+        <v>Expected</v>
+      </c>
+      <c r="G1" t="str">
+        <v/>
+      </c>
+      <c r="H1" t="str">
+        <v/>
+      </c>
+      <c r="I1" t="str">
+        <v/>
+      </c>
+      <c r="J1" t="str">
+        <v/>
+      </c>
+      <c r="K1" t="str">
+        <v/>
+      </c>
+      <c r="L1" t="str">
+        <v/>
+      </c>
+      <c r="M1" t="str">
+        <v/>
+      </c>
+      <c r="N1" t="str">
+        <v/>
+      </c>
+      <c r="O1" t="str">
+        <v/>
+      </c>
+      <c r="P1" t="str">
+        <v/>
+      </c>
+      <c r="Q1" t="str">
+        <v/>
+      </c>
+      <c r="R1" t="str">
+        <v/>
+      </c>
+      <c r="S1" t="str">
+        <v/>
+      </c>
+      <c r="T1" t="str">
+        <v/>
+      </c>
+      <c r="U1" t="str">
+        <v/>
+      </c>
+      <c r="V1" t="str">
+        <v/>
+      </c>
+      <c r="W1" t="str">
+        <v/>
+      </c>
+      <c r="X1" t="str">
+        <v/>
+      </c>
+      <c r="Y1" t="str">
+        <v/>
+      </c>
+      <c r="Z1" t="str">
+        <v>_x000d_</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>User successfully completed profile setup</v>
+      </c>
+      <c r="B2" t="str">
+        <v>new@gmail.com</v>
+      </c>
+      <c r="C2" t="str">
+        <v>New Man</v>
+      </c>
+      <c r="D2" t="str">
+        <v>Newman</v>
+      </c>
+      <c r="E2" t="str">
+        <v>newman@123</v>
+      </c>
+      <c r="F2" t="str">
+        <v>For Background</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>Verify supported file types (PDF) in blood report upload modal</v>
+      </c>
+      <c r="F3" t="str">
+        <v>Only PDF files are supported</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>Verify file size limit (10MB) in blood report upload modal</v>
+      </c>
+      <c r="F4" t="str">
+        <v>Supports PDF files (max 10MB)</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:Z4"/>
+  </ignoredErrors>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updated onboarding scenarios with report and added subfolders for feature files
</commit_message>
<xml_diff>
--- a/testData/testData.xlsx
+++ b/testData/testData.xlsx
@@ -5052,7 +5052,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Z4"/>
+  <dimension ref="A1:Z5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -5173,9 +5173,17 @@
         <v>Supports PDF files (max 10MB)</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>Verify incomplete steps (2-5) are not highlighted in report analysis</v>
+      </c>
+      <c r="F5" t="str">
+        <v>bg-purple-200/50</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:Z4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:Z5"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>